<commit_message>
revise comment in app.js
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -490,10 +490,21 @@
         <v>04-10-2023</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>test test test 4 10</v>
+      </c>
+      <c r="C9" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update the comment system
Add the comment-list area to show the most recent comments up to 5.
And after the user submitted the comment. the comments will be shown automatically
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -424,9 +424,189 @@
         <v>04-10-2023</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>test again</v>
+      </c>
+      <c r="C3" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>test 3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <v>test 4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">test 5 </v>
+      </c>
+      <c r="C6" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <v>test 6</v>
+      </c>
+      <c r="C7" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str" xml:space="preserve">
+        <v xml:space="preserve">tst test 6
+</v>
+      </c>
+      <c r="C8" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>test 7</v>
+      </c>
+      <c r="C9" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str" xml:space="preserve">
+        <v xml:space="preserve">new test
+</v>
+      </c>
+      <c r="C10" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <v>new try</v>
+      </c>
+      <c r="C11" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="str">
+        <v>eferere</v>
+      </c>
+      <c r="C12" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="str">
+        <v>just test test</v>
+      </c>
+      <c r="C13" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="str">
+        <v>treestesfdsaete</v>
+      </c>
+      <c r="C14" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="str">
+        <v>most recent comments</v>
+      </c>
+      <c r="C15" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="16" xml:space="preserve">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="str" xml:space="preserve">
+        <v xml:space="preserve">jdslkfdsa er erakldf erkajfd aekrejalks dfjsalkre
+a ereal;rkesa;skrjeas 
+ae r;alsejres</v>
+      </c>
+      <c r="C16" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="str">
+        <v>tstest</v>
+      </c>
+      <c r="C17" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="str">
+        <v xml:space="preserve">nice test </v>
+      </c>
+      <c r="C18" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update a small error in submitCommnet.js
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -615,9 +615,20 @@
         <v>04-10-2023</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="str">
+        <v>test</v>
+      </c>
+      <c r="C20" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change the CSS style for comments
Now, the bottom of each comment will show ID at left side and Time at right side.
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -626,9 +626,64 @@
         <v>04-10-2023</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="str">
+        <v>let us test the comment system</v>
+      </c>
+      <c r="C21" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="str">
+        <v>test again</v>
+      </c>
+      <c r="C22" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="str">
+        <v xml:space="preserve">test it </v>
+      </c>
+      <c r="C23" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="str">
+        <v>this ID should be 22</v>
+      </c>
+      <c r="C24" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="str">
+        <v>test 23</v>
+      </c>
+      <c r="C25" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changing the color of ID and Time
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -681,9 +681,31 @@
         <v>04-10-2023</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="str">
+        <v>I like this garden</v>
+      </c>
+      <c r="C26" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="str">
+        <v>test id should be 25</v>
+      </c>
+      <c r="C27" t="str">
+        <v>04-10-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the express-rate-limit package
Now, user can only submit one comment in every two minutes
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -703,9 +703,42 @@
         <v>04-10-2023</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="str">
+        <v>test test</v>
+      </c>
+      <c r="C28" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="str">
+        <v>test again</v>
+      </c>
+      <c r="C29" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="str">
+        <v>test</v>
+      </c>
+      <c r="C30" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C30"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set the limitation of submission
3 submission in 2 minutes
add the Googel reCaptcha for submission
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -736,9 +736,86 @@
         <v>04-11-2023</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="str">
+        <v>test again</v>
+      </c>
+      <c r="C31" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="str">
+        <v>rewr</v>
+      </c>
+      <c r="C32" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="str">
+        <v>sawewe</v>
+      </c>
+      <c r="C33" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="str">
+        <v>erwerewrw</v>
+      </c>
+      <c r="C34" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="str">
+        <v>ewrwer</v>
+      </c>
+      <c r="C35" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="str">
+        <v>wewqe</v>
+      </c>
+      <c r="C36" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="str">
+        <v>dfsfsdfsfsd</v>
+      </c>
+      <c r="C37" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C37"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set the map bound
The users will be restricted in the map  area of UNC campus
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -813,9 +813,20 @@
         <v>04-11-2023</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="str">
+        <v>dsfdsfsd</v>
+      </c>
+      <c r="C38" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C37"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C38"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set the maxzoom to 14
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -824,9 +824,53 @@
         <v>04-11-2023</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="str">
+        <v>erwrewrw</v>
+      </c>
+      <c r="C39" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="str">
+        <v>erwerwrew</v>
+      </c>
+      <c r="C40" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="str">
+        <v>dfdsfsfs</v>
+      </c>
+      <c r="C41" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="str">
+        <v>erwrwerw</v>
+      </c>
+      <c r="C42" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C42"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
make the restricted map area bigger
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -901,9 +901,53 @@
         <v>04-11-2023</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="str">
+        <v>test test</v>
+      </c>
+      <c r="C46" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="str">
+        <v>test again</v>
+      </c>
+      <c r="C47" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="str">
+        <v>testestes</v>
+      </c>
+      <c r="C48" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="str">
+        <v>tstest</v>
+      </c>
+      <c r="C49" t="str">
+        <v>04-11-2023</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C45"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C49"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix the invalid date for comment in firefox
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -989,9 +989,53 @@
         <v>04-13-2023</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="str">
+        <v>fdgrt</v>
+      </c>
+      <c r="C54" t="str">
+        <v>04-14-2023</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="str">
+        <v>sawesda</v>
+      </c>
+      <c r="C55" t="str">
+        <v>2023-04-15T01:50:48.080Z</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="str">
+        <v>ersdfs</v>
+      </c>
+      <c r="C56" t="str">
+        <v>2023-04-15T01:52:14.613Z</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="str">
+        <v>qwewqe</v>
+      </c>
+      <c r="C57" t="str">
+        <v>2023-04-15T01:52:44.738Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C53"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C57"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementation of showing plants for each garden by read the excel file
</commit_message>
<xml_diff>
--- a/comments/comments.xlsx
+++ b/comments/comments.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -484,7 +484,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">tst test 6
+        <v xml:space="preserve">tst test 6_x000d_
 </v>
       </c>
       <c r="C8" t="str">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">new test
+        <v xml:space="preserve">new test_x000d_
 </v>
       </c>
       <c r="C10" t="str">
@@ -525,58 +525,25 @@
         <v>04-10-2023</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="str">
-        <v>eferere</v>
-      </c>
-      <c r="C12" t="str">
-        <v>04-10-2023</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="str">
-        <v>just test test</v>
-      </c>
-      <c r="C13" t="str">
-        <v>04-10-2023</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="str">
-        <v>treestesfdsaete</v>
-      </c>
-      <c r="C14" t="str">
-        <v>04-10-2023</v>
-      </c>
-    </row>
-    <row r="15">
+    <row r="15" xml:space="preserve">
       <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="str">
-        <v>most recent comments</v>
+        <v>14</v>
+      </c>
+      <c r="B15" t="str" xml:space="preserve">
+        <v xml:space="preserve">jdslkfdsa er erakldf erkajfd aekrejalks dfjsalkre_x000d_
+a ereal;rkesa;skrjeas _x000d_
+ae r;alsejres</v>
       </c>
       <c r="C15" t="str">
         <v>04-10-2023</v>
       </c>
     </row>
-    <row r="16" xml:space="preserve">
+    <row r="16">
       <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="str" xml:space="preserve">
-        <v xml:space="preserve">jdslkfdsa er erakldf erkajfd aekrejalks dfjsalkre
-a ereal;rkesa;skrjeas 
-ae r;alsejres</v>
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>tstest</v>
       </c>
       <c r="C16" t="str">
         <v>04-10-2023</v>
@@ -584,10 +551,10 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="str">
-        <v>tstest</v>
+        <v xml:space="preserve">nice test </v>
       </c>
       <c r="C17" t="str">
         <v>04-10-2023</v>
@@ -595,10 +562,10 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="str">
-        <v xml:space="preserve">nice test </v>
+        <v>I like this garden. The plants look great.</v>
       </c>
       <c r="C18" t="str">
         <v>04-10-2023</v>
@@ -606,10 +573,10 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="str">
-        <v>I like this garden. The plants look great.</v>
+        <v>test</v>
       </c>
       <c r="C19" t="str">
         <v>04-10-2023</v>
@@ -617,10 +584,10 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="str">
-        <v>test</v>
+        <v>let us test the comment system</v>
       </c>
       <c r="C20" t="str">
         <v>04-10-2023</v>
@@ -628,10 +595,10 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="str">
-        <v>let us test the comment system</v>
+        <v>test again</v>
       </c>
       <c r="C21" t="str">
         <v>04-10-2023</v>
@@ -639,10 +606,10 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="str">
-        <v>test again</v>
+        <v xml:space="preserve">test it </v>
       </c>
       <c r="C22" t="str">
         <v>04-10-2023</v>
@@ -650,10 +617,10 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="str">
-        <v xml:space="preserve">test it </v>
+        <v>this ID should be 22</v>
       </c>
       <c r="C23" t="str">
         <v>04-10-2023</v>
@@ -661,10 +628,10 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="str">
-        <v>this ID should be 22</v>
+        <v>test 23</v>
       </c>
       <c r="C24" t="str">
         <v>04-10-2023</v>
@@ -672,10 +639,10 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="str">
-        <v>test 23</v>
+        <v>I like this garden</v>
       </c>
       <c r="C25" t="str">
         <v>04-10-2023</v>
@@ -683,10 +650,10 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="str">
-        <v>I like this garden</v>
+        <v>test id should be 25</v>
       </c>
       <c r="C26" t="str">
         <v>04-10-2023</v>
@@ -694,21 +661,21 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="str">
-        <v>test id should be 25</v>
+        <v>test test</v>
       </c>
       <c r="C27" t="str">
-        <v>04-10-2023</v>
+        <v>04-11-2023</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="str">
-        <v>test test</v>
+        <v>test again</v>
       </c>
       <c r="C28" t="str">
         <v>04-11-2023</v>
@@ -716,10 +683,10 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="str">
-        <v>test again</v>
+        <v>test</v>
       </c>
       <c r="C29" t="str">
         <v>04-11-2023</v>
@@ -727,10 +694,10 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="str">
-        <v>test</v>
+        <v>test again</v>
       </c>
       <c r="C30" t="str">
         <v>04-11-2023</v>
@@ -738,10 +705,10 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="str">
-        <v>test again</v>
+        <v>rewr</v>
       </c>
       <c r="C31" t="str">
         <v>04-11-2023</v>
@@ -749,10 +716,10 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="str">
-        <v>rewr</v>
+        <v>sawewe</v>
       </c>
       <c r="C32" t="str">
         <v>04-11-2023</v>
@@ -760,10 +727,10 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="str">
-        <v>sawewe</v>
+        <v>erwerewrw</v>
       </c>
       <c r="C33" t="str">
         <v>04-11-2023</v>
@@ -771,10 +738,10 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="str">
-        <v>erwerewrw</v>
+        <v>ewrwer</v>
       </c>
       <c r="C34" t="str">
         <v>04-11-2023</v>
@@ -782,10 +749,10 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="str">
-        <v>ewrwer</v>
+        <v>wewqe</v>
       </c>
       <c r="C35" t="str">
         <v>04-11-2023</v>
@@ -793,10 +760,10 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="str">
-        <v>wewqe</v>
+        <v>dfsfsdfsfsd</v>
       </c>
       <c r="C36" t="str">
         <v>04-11-2023</v>
@@ -804,10 +771,10 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="str">
-        <v>dfsfsdfsfsd</v>
+        <v>dsfdsfsd</v>
       </c>
       <c r="C37" t="str">
         <v>04-11-2023</v>
@@ -815,10 +782,10 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="str">
-        <v>dsfdsfsd</v>
+        <v>erwrewrw</v>
       </c>
       <c r="C38" t="str">
         <v>04-11-2023</v>
@@ -826,10 +793,10 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="str">
-        <v>erwrewrw</v>
+        <v>erwerwrew</v>
       </c>
       <c r="C39" t="str">
         <v>04-11-2023</v>
@@ -837,10 +804,10 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="str">
-        <v>erwerwrew</v>
+        <v>dfdsfsfs</v>
       </c>
       <c r="C40" t="str">
         <v>04-11-2023</v>
@@ -848,10 +815,10 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="str">
-        <v>dfdsfsfs</v>
+        <v>erwrwerw</v>
       </c>
       <c r="C41" t="str">
         <v>04-11-2023</v>
@@ -859,10 +826,10 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="str">
-        <v>erwrwerw</v>
+        <v>rewrwer</v>
       </c>
       <c r="C42" t="str">
         <v>04-11-2023</v>
@@ -870,10 +837,10 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="str">
-        <v>rewrwer</v>
+        <v>tertertre</v>
       </c>
       <c r="C43" t="str">
         <v>04-11-2023</v>
@@ -881,10 +848,10 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="str">
-        <v>tertertre</v>
+        <v>rewrwe</v>
       </c>
       <c r="C44" t="str">
         <v>04-11-2023</v>
@@ -892,10 +859,10 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="str">
-        <v>rewrwe</v>
+        <v>test test</v>
       </c>
       <c r="C45" t="str">
         <v>04-11-2023</v>
@@ -903,10 +870,10 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="str">
-        <v>test test</v>
+        <v>test again</v>
       </c>
       <c r="C46" t="str">
         <v>04-11-2023</v>
@@ -914,10 +881,10 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="str">
-        <v>test again</v>
+        <v>testestes</v>
       </c>
       <c r="C47" t="str">
         <v>04-11-2023</v>
@@ -925,10 +892,10 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="str">
-        <v>testestes</v>
+        <v>tstest</v>
       </c>
       <c r="C48" t="str">
         <v>04-11-2023</v>
@@ -936,10 +903,10 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="str">
-        <v>tstest</v>
+        <v>test</v>
       </c>
       <c r="C49" t="str">
         <v>04-11-2023</v>
@@ -947,10 +914,10 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" t="str">
-        <v>test</v>
+        <v>test test</v>
       </c>
       <c r="C50" t="str">
         <v>04-11-2023</v>
@@ -958,84 +925,108 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" t="str">
-        <v>test test</v>
+        <v>test</v>
       </c>
       <c r="C51" t="str">
-        <v>04-11-2023</v>
+        <v>04-12-2023</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" t="str">
-        <v>test</v>
+        <v>i7ryuk</v>
       </c>
       <c r="C52" t="str">
-        <v>04-12-2023</v>
+        <v>04-13-2023</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" t="str">
-        <v>i7ryuk</v>
+        <v>fdgrt</v>
       </c>
       <c r="C53" t="str">
-        <v>04-13-2023</v>
+        <v>04-14-2023</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" t="str">
-        <v>fdgrt</v>
+        <v>sawesda</v>
       </c>
       <c r="C54" t="str">
-        <v>04-14-2023</v>
+        <v>2023-04-15T01:50:48.080Z</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" t="str">
-        <v>sawesda</v>
+        <v>ersdfs</v>
       </c>
       <c r="C55" t="str">
-        <v>2023-04-15T01:50:48.080Z</v>
+        <v>2023-04-15T01:52:14.613Z</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" t="str">
-        <v>ersdfs</v>
+        <v>qwewqe</v>
       </c>
       <c r="C56" t="str">
-        <v>2023-04-15T01:52:14.613Z</v>
+        <v>2023-04-15T01:52:44.738Z</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" t="str">
-        <v>qwewqe</v>
+        <v>ersdfas</v>
       </c>
       <c r="C57" t="str">
-        <v>2023-04-15T01:52:44.738Z</v>
+        <v>04-14-2023</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="str">
+        <v>ewrwwerwe</v>
+      </c>
+      <c r="C58" t="str">
+        <v>2023-04-15T02:14:09.711Z</v>
+      </c>
+    </row>
+    <row r="60" xml:space="preserve">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="str" xml:space="preserve">
+        <v xml:space="preserve">test testtest
+</v>
+      </c>
+      <c r="C60" t="str">
+        <v>2023-04-15T19:51:43.709Z</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C57"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C60"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>